<commit_message>
Saving corrected data with new parameters as csv
</commit_message>
<xml_diff>
--- a/data/originalData/fieldDataRaw.xlsx
+++ b/data/originalData/fieldDataRaw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Charlotte\Data collection\IRGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acole\Documents\R_Files\dissertation\data\originalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_01B5AD203028809475AFB5E5008C7A043C6D6101" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8507CCD-FA5B-4346-B847-CD8802DE46E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB74CD5-1120-41DE-BBC5-C0B8020F1AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19400" windowHeight="7390" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chorisodontium" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,12 +604,12 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -850,7 +850,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -969,7 +969,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44959</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44961</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44963</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44964</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44965</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44966</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44970</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>142.85</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44971</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>136.66</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>153.13999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>146.28</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44972</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>141.13</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>133.88</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44973</v>
       </c>
@@ -5634,9 +5634,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44959</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44961</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -9209,7 +9209,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44963</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44964</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -9566,7 +9566,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44965</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44966</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44970</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>106.37</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44971</v>
       </c>
@@ -10131,7 +10131,7 @@
         <v>103.12</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>113.98</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -10339,7 +10339,7 @@
         <v>109.57</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44972</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>106.67</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>102.47</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44973</v>
       </c>
@@ -10664,9 +10664,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10788,7 +10788,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16.5">
+    <row r="2" spans="1:40" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -11383,7 +11383,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -11502,7 +11502,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -11621,7 +11621,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -11740,7 +11740,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -11859,7 +11859,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -11978,7 +11978,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -12335,7 +12335,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -12573,7 +12573,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -12692,7 +12692,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -12811,7 +12811,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -12930,7 +12930,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -13168,7 +13168,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -13287,7 +13287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -13406,7 +13406,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -13525,7 +13525,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -13763,7 +13763,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44961</v>
       </c>
@@ -13882,7 +13882,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -14001,7 +14001,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44963</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -14239,7 +14239,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44964</v>
       </c>
@@ -14358,7 +14358,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44965</v>
       </c>
@@ -14477,7 +14477,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -14596,7 +14596,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44966</v>
       </c>
@@ -14715,7 +14715,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -14834,7 +14834,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44970</v>
       </c>
@@ -14938,7 +14938,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44971</v>
       </c>
@@ -15042,7 +15042,7 @@
         <v>18.41</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44972</v>
       </c>
@@ -15146,7 +15146,7 @@
         <v>19.63</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -15250,7 +15250,7 @@
         <v>17.18</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -15354,7 +15354,7 @@
         <v>15.95</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44973</v>
       </c>
@@ -15458,7 +15458,7 @@
         <v>14.85</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -15562,7 +15562,7 @@
         <v>14.17</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44975</v>
       </c>
@@ -15679,9 +15679,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15803,7 +15803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16.5">
+    <row r="2" spans="1:40" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -15922,7 +15922,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -16041,7 +16041,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -16160,7 +16160,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -16279,7 +16279,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -16398,7 +16398,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -16517,7 +16517,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -16636,7 +16636,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -16755,7 +16755,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -16874,7 +16874,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -16993,7 +16993,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -17112,7 +17112,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -17231,7 +17231,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -17350,7 +17350,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -17469,7 +17469,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -17588,7 +17588,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -17707,7 +17707,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -17826,7 +17826,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -17945,7 +17945,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -18064,7 +18064,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -18183,7 +18183,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -18302,7 +18302,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -18421,7 +18421,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -18540,7 +18540,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -18659,7 +18659,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -18778,7 +18778,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44961</v>
       </c>
@@ -18897,7 +18897,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -19016,7 +19016,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44963</v>
       </c>
@@ -19135,7 +19135,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -19254,7 +19254,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44964</v>
       </c>
@@ -19373,7 +19373,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44965</v>
       </c>
@@ -19492,7 +19492,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -19611,7 +19611,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44966</v>
       </c>
@@ -19730,7 +19730,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -19849,7 +19849,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44970</v>
       </c>
@@ -19953,7 +19953,7 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44971</v>
       </c>
@@ -20057,7 +20057,7 @@
         <v>8.68</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44972</v>
       </c>
@@ -20161,7 +20161,7 @@
         <v>10.71</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -20265,7 +20265,7 @@
         <v>9.57</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -20369,7 +20369,7 @@
         <v>8.73</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44973</v>
       </c>
@@ -20473,7 +20473,7 @@
         <v>7.76</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -20577,7 +20577,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44975</v>
       </c>
@@ -20694,9 +20694,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20818,7 +20818,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16.5">
+    <row r="2" spans="1:40" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -20937,7 +20937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -21056,7 +21056,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -21175,7 +21175,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -21294,7 +21294,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -21413,7 +21413,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -21532,7 +21532,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -21651,7 +21651,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -21770,7 +21770,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -21889,7 +21889,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -22008,7 +22008,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -22127,7 +22127,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -22246,7 +22246,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -22365,7 +22365,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -22484,7 +22484,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -22603,7 +22603,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -22722,7 +22722,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -22841,7 +22841,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -22960,7 +22960,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -23079,7 +23079,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -23198,7 +23198,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -23317,7 +23317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -23436,7 +23436,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -23555,7 +23555,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -23674,7 +23674,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -23793,7 +23793,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44961</v>
       </c>
@@ -23912,7 +23912,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -24031,7 +24031,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44963</v>
       </c>
@@ -24150,7 +24150,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -24269,7 +24269,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44964</v>
       </c>
@@ -24388,7 +24388,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44965</v>
       </c>
@@ -24507,7 +24507,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -24626,7 +24626,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44966</v>
       </c>
@@ -24745,7 +24745,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -24864,7 +24864,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44970</v>
       </c>
@@ -24968,7 +24968,7 @@
         <v>6.53</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44971</v>
       </c>
@@ -25072,7 +25072,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44972</v>
       </c>
@@ -25176,7 +25176,7 @@
         <v>6.42</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -25280,7 +25280,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -25384,7 +25384,7 @@
         <v>6.03</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44973</v>
       </c>
@@ -25488,7 +25488,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -25592,7 +25592,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44975</v>
       </c>
@@ -25709,9 +25709,9 @@
       <selection activeCell="AO20" sqref="AO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -25833,7 +25833,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16.5">
+    <row r="2" spans="1:40" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -25952,7 +25952,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -26071,7 +26071,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -26190,7 +26190,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -26309,7 +26309,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -26428,7 +26428,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -26547,7 +26547,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -26666,7 +26666,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -26785,7 +26785,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -26904,7 +26904,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -27023,7 +27023,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -27142,7 +27142,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -27261,7 +27261,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -27380,7 +27380,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -27499,7 +27499,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -27618,7 +27618,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -27737,7 +27737,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -27856,7 +27856,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -27978,7 +27978,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:41">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -28097,7 +28097,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="21" spans="1:41">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -28216,7 +28216,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:41">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -28335,7 +28335,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:41">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -28454,7 +28454,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="24" spans="1:41">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -28573,7 +28573,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="25" spans="1:41">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -28692,7 +28692,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:41">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -28811,7 +28811,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="27" spans="1:41">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44961</v>
       </c>
@@ -28930,7 +28930,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -29049,7 +29049,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="29" spans="1:41">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44963</v>
       </c>
@@ -29168,7 +29168,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="30" spans="1:41">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -29287,7 +29287,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="31" spans="1:41">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44964</v>
       </c>
@@ -29406,7 +29406,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="32" spans="1:41">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44965</v>
       </c>
@@ -29525,7 +29525,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -29644,7 +29644,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44966</v>
       </c>
@@ -29763,7 +29763,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -29882,7 +29882,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44970</v>
       </c>
@@ -29986,7 +29986,7 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44971</v>
       </c>
@@ -30090,7 +30090,7 @@
         <v>12.59</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44972</v>
       </c>
@@ -30194,7 +30194,7 @@
         <v>12.83</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -30298,7 +30298,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -30402,7 +30402,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44973</v>
       </c>
@@ -30506,7 +30506,7 @@
         <v>11.58</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -30610,7 +30610,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44975</v>
       </c>
@@ -30724,15 +30724,15 @@
   <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -30854,7 +30854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16.5">
+    <row r="2" spans="1:40" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -30973,7 +30973,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -31092,7 +31092,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -31211,7 +31211,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -31330,7 +31330,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -31449,7 +31449,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -31568,7 +31568,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -31687,7 +31687,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -31806,7 +31806,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -31925,7 +31925,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -32044,7 +32044,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -32163,7 +32163,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -32282,7 +32282,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -32401,7 +32401,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -32520,7 +32520,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -32639,7 +32639,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -32758,7 +32758,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -32877,7 +32877,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -32996,7 +32996,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -33115,7 +33115,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -33234,7 +33234,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -33353,7 +33353,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -33472,7 +33472,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -33591,7 +33591,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -33710,7 +33710,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -33829,7 +33829,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44961</v>
       </c>
@@ -33948,7 +33948,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -34067,7 +34067,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44963</v>
       </c>
@@ -34186,7 +34186,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -34305,7 +34305,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44964</v>
       </c>
@@ -34424,7 +34424,7 @@
         <v>5.54</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44965</v>
       </c>
@@ -34543,7 +34543,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -34662,7 +34662,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44966</v>
       </c>
@@ -34781,7 +34781,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -34900,7 +34900,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44970</v>
       </c>
@@ -35004,7 +35004,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44971</v>
       </c>
@@ -35108,7 +35108,7 @@
         <v>11.27</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44972</v>
       </c>
@@ -35212,7 +35212,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -35316,7 +35316,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -35420,7 +35420,7 @@
         <v>10.71</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44973</v>
       </c>
@@ -35524,7 +35524,7 @@
         <v>10.55</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -35628,7 +35628,7 @@
         <v>10.61</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44975</v>
       </c>
@@ -35745,9 +35745,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -35869,7 +35869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16.5">
+    <row r="2" spans="1:40" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -35988,7 +35988,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44931</v>
       </c>
@@ -36107,7 +36107,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44933</v>
       </c>
@@ -36226,7 +36226,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44935</v>
       </c>
@@ -36345,7 +36345,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44938</v>
       </c>
@@ -36464,7 +36464,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44938</v>
       </c>
@@ -36583,7 +36583,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44940</v>
       </c>
@@ -36702,7 +36702,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44940</v>
       </c>
@@ -36821,7 +36821,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44941</v>
       </c>
@@ -36940,7 +36940,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44941</v>
       </c>
@@ -37059,7 +37059,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44943</v>
       </c>
@@ -37178,7 +37178,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44944</v>
       </c>
@@ -37297,7 +37297,7 @@
         <v>11.58</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44944</v>
       </c>
@@ -37416,7 +37416,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44945</v>
       </c>
@@ -37535,7 +37535,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44947</v>
       </c>
@@ -37654,7 +37654,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44948</v>
       </c>
@@ -37773,7 +37773,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44948</v>
       </c>
@@ -37892,7 +37892,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44950</v>
       </c>
@@ -38011,7 +38011,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44953</v>
       </c>
@@ -38130,7 +38130,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44953</v>
       </c>
@@ -38249,7 +38249,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44953</v>
       </c>
@@ -38368,7 +38368,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44956</v>
       </c>
@@ -38487,7 +38487,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44956</v>
       </c>
@@ -38606,7 +38606,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44958</v>
       </c>
@@ -38725,7 +38725,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44959</v>
       </c>
@@ -38844,7 +38844,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44961</v>
       </c>
@@ -38963,7 +38963,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44961</v>
       </c>
@@ -39082,7 +39082,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44963</v>
       </c>
@@ -39201,7 +39201,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>44963</v>
       </c>
@@ -39320,7 +39320,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>44964</v>
       </c>
@@ -39439,7 +39439,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>44965</v>
       </c>
@@ -39558,7 +39558,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>44965</v>
       </c>
@@ -39677,7 +39677,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>44966</v>
       </c>
@@ -39796,7 +39796,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>44966</v>
       </c>
@@ -39915,7 +39915,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>44970</v>
       </c>
@@ -40019,7 +40019,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>44971</v>
       </c>
@@ -40123,7 +40123,7 @@
         <v>7.51</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>44972</v>
       </c>
@@ -40227,7 +40227,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>44972</v>
       </c>
@@ -40331,7 +40331,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>44972</v>
       </c>
@@ -40435,7 +40435,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44973</v>
       </c>
@@ -40539,7 +40539,7 @@
         <v>7.08</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44973</v>
       </c>
@@ -40643,7 +40643,7 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44975</v>
       </c>
@@ -40759,6 +40759,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3A510C09EC0784C97ED39A831708B55" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dcd91ea404c6446efeaf4806639ff170">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="be0714b7-0736-4a3e-b286-5892629adf2b" xmlns:ns3="75d2bd05-bfc3-4ab3-a6a4-92e3ad8ab906" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2dd77ba40112074ce522464c1bc3ad8" ns2:_="" ns3:_="">
     <xsd:import namespace="be0714b7-0736-4a3e-b286-5892629adf2b"/>
@@ -40923,23 +40932,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB07F615-DCC8-4199-9E0F-7900573F825F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB07F615-DCC8-4199-9E0F-7900573F825F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B24FD3-7239-42D3-8C0A-EBE5A37F21C6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4996BAC6-55BB-4095-8C56-4CA6AC61DC05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4996BAC6-55BB-4095-8C56-4CA6AC61DC05}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B24FD3-7239-42D3-8C0A-EBE5A37F21C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0714b7-0736-4a3e-b286-5892629adf2b"/>
+    <ds:schemaRef ds:uri="75d2bd05-bfc3-4ab3-a6a4-92e3ad8ab906"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>